<commit_message>
Adding write2 to make the wafferPlan in a csv
</commit_message>
<xml_diff>
--- a/dataset/Hackaton DB Final 04.21.xlsx
+++ b/dataset/Hackaton DB Final 04.21.xlsx
@@ -1198,7 +1198,7 @@
         <v>5564396250</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>5564485886.189131</v>
+        <v>5564485886.18913</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>5564490050.576762</v>
@@ -1210,7 +1210,7 @@
         <v>4785461369.891063</v>
       </c>
       <c r="K2" s="4" t="n">
-        <v>4785461946.930285</v>
+        <v>4785461946.930284</v>
       </c>
       <c r="L2" s="4" t="n">
         <v>4785406272.929749</v>
@@ -1583,13 +1583,13 @@
         <v>2681843296.107904</v>
       </c>
       <c r="G6" s="4" t="n">
-        <v>4824136388.976886</v>
+        <v>4824136388.976885</v>
       </c>
       <c r="H6" s="4" t="n">
-        <v>3360541781.413641</v>
+        <v>3360541781.41364</v>
       </c>
       <c r="I6" s="4" t="n">
-        <v>6503118573.213696</v>
+        <v>6503118573.213695</v>
       </c>
       <c r="J6" s="4" t="n">
         <v>10344070194.5533</v>
@@ -1746,7 +1746,7 @@
         <v>916289416.3499999</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>2129234704.355187</v>
+        <v>2129234704.355186</v>
       </c>
       <c r="G8" s="4" t="n">
         <v>1256964727.075411</v>
@@ -1755,7 +1755,7 @@
         <v>2046159316.690736</v>
       </c>
       <c r="I8" s="4" t="n">
-        <v>2203542654.663653</v>
+        <v>2203542654.663652</v>
       </c>
       <c r="J8" s="4" t="n">
         <v>1479523540.134121</v>
@@ -2157,31 +2157,31 @@
         <v>536624401.5999999</v>
       </c>
       <c r="F12" s="4" t="n">
-        <v>353027431.6551874</v>
+        <v>353027431.6551871</v>
       </c>
       <c r="G12" s="4" t="n">
-        <v>368128099.3548417</v>
+        <v>368128099.3548412</v>
       </c>
       <c r="H12" s="4" t="n">
-        <v>-245814176.2140052</v>
+        <v>-245814176.2140055</v>
       </c>
       <c r="I12" s="4" t="n">
-        <v>368864309.3945987</v>
+        <v>368864309.394598</v>
       </c>
       <c r="J12" s="4" t="n">
-        <v>368580775.4913361</v>
+        <v>368580775.4913354</v>
       </c>
       <c r="K12" s="4" t="n">
-        <v>342846281.304709</v>
+        <v>342846281.3047082</v>
       </c>
       <c r="L12" s="4" t="n">
-        <v>308970980.6662872</v>
+        <v>308970980.6662865</v>
       </c>
       <c r="M12" s="4" t="n">
-        <v>-601203031.6505203</v>
+        <v>-601203031.6505208</v>
       </c>
       <c r="N12" s="4" t="n">
-        <v>177252124.5571055</v>
+        <v>177252124.5571051</v>
       </c>
       <c r="O12" s="4" t="n">
         <v>2005693964.442241</v>
@@ -2275,28 +2275,28 @@
         <v>139999981.4699614</v>
       </c>
       <c r="G13" s="12" t="n">
-        <v>139973232.0187311</v>
+        <v>139973232.0187309</v>
       </c>
       <c r="H13" s="12" t="n">
-        <v>-4610684124.748766</v>
+        <v>-4610684124.748768</v>
       </c>
       <c r="I13" s="12" t="n">
-        <v>133152182.6015007</v>
+        <v>133152182.6015005</v>
       </c>
       <c r="J13" s="12" t="n">
-        <v>139962148.383188</v>
+        <v>139962148.3831873</v>
       </c>
       <c r="K13" s="12" t="n">
-        <v>139776569.505137</v>
+        <v>139776569.505136</v>
       </c>
       <c r="L13" s="12" t="n">
-        <v>139929049.1730887</v>
+        <v>139929049.1730878</v>
       </c>
       <c r="M13" s="12" t="n">
-        <v>-4839390807.755149</v>
+        <v>-4839390807.75515</v>
       </c>
       <c r="N13" s="12" t="n">
-        <v>139903893.1295946</v>
+        <v>139903893.1295941</v>
       </c>
       <c r="O13" s="12" t="n">
         <v>-2116106065.447186</v>
@@ -2346,7 +2346,7 @@
         <v>2038937754.98</v>
       </c>
       <c r="E14" s="4" t="n">
-        <v>5590446425.865001</v>
+        <v>5590446425.865</v>
       </c>
       <c r="F14" s="4" t="n">
         <v>4012105699</v>
@@ -2358,7 +2358,7 @@
         <v>3534484566.201103</v>
       </c>
       <c r="I14" s="4" t="n">
-        <v>738135162.0752832</v>
+        <v>738135162.0752831</v>
       </c>
       <c r="J14" s="4" t="n">
         <v>938256007.8486817</v>
@@ -2373,7 +2373,7 @@
         <v>393462387.4999999</v>
       </c>
       <c r="N14" s="4" t="n">
-        <v>794794022.75</v>
+        <v>794794022.7499999</v>
       </c>
       <c r="O14" s="4" t="n">
         <v>393462387.4999999</v>
@@ -2418,7 +2418,7 @@
         <v>3534502893.25</v>
       </c>
       <c r="AC14" s="0" t="n">
-        <v>707869101.45</v>
+        <v>707869101.4499999</v>
       </c>
       <c r="AD14" s="0" t="n">
         <v>2911621667.5</v>
@@ -2430,7 +2430,7 @@
         <v>3534502893.25</v>
       </c>
       <c r="AG14" s="0" t="n">
-        <v>707869101.45</v>
+        <v>707869101.4499999</v>
       </c>
       <c r="AH14" s="0" t="n">
         <v>2911621667.5</v>
@@ -2442,7 +2442,7 @@
         <v>3534502893.25</v>
       </c>
       <c r="AK14" s="0" t="n">
-        <v>707869101.45</v>
+        <v>707869101.4499999</v>
       </c>
     </row>
     <row r="15" ht="10.5" customHeight="1" s="71">
@@ -2754,10 +2754,10 @@
         <v>184132359.936</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>-2482425490.991282</v>
+        <v>-2482425490.991281</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>-3359971328.792211</v>
+        <v>-3359971328.79221</v>
       </c>
       <c r="F18" s="4" t="n">
         <v>-5214942541.272617</v>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="D19" s="12" t="n"/>
       <c r="E19" s="12" t="n">
-        <v>-15488622758.53059</v>
+        <v>-15488622758.53058</v>
       </c>
       <c r="F19" s="12" t="n">
         <v>-14494470066.84175</v>
@@ -2929,7 +2929,9 @@
       <c r="AH19" s="0" t="n"/>
       <c r="AI19" s="0" t="n"/>
       <c r="AJ19" s="0" t="n"/>
-      <c r="AK19" s="0" t="n"/>
+      <c r="AK19" s="0" t="n">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>